<commit_message>
figures after 85% data collected
</commit_message>
<xml_diff>
--- a/xlsx/country_comparison/.xlsx
+++ b/xlsx/country_comparison/.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -32,31 +32,49 @@
     <t xml:space="preserve">United States</t>
   </si>
   <si>
-    <t xml:space="preserve">Conjoint: &gt;&gt;C+NR+GCS&lt;&lt; vs. C+NR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conjoint: C+NR vs. &gt;&gt;GCS+NR&lt;&lt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conjoint: NR vs. &gt;&gt;NR+C+GCS&lt;&lt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conjoint: &gt;&gt;NR+GCS&lt;&lt; vs. NR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conjoint: &gt;&gt;NR+C&lt;&lt; vs. NR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conjoint: &gt;&gt;Left&lt;&lt; vs. Right</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conjoint: &gt;&gt;Left+GCS&lt;&lt; vs. Right</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conjoint: random programs &gt;&gt;A&lt;&lt; vs. B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conjoint: random programs &gt;&gt;A+GCS&lt;&lt; vs. B</t>
+    <t xml:space="preserve">econ1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">econ2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">econ3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">econ4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soc1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soc2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">climate1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">climate2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">climate3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax1: National redistribution scheme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax2: Wealth tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foreign1: Global climate scheme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foreign2: Global tax on millionaires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foreign3: Global democratic assembly on climate change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foreign4: Doubling foreign aid</t>
   </si>
 </sst>
 </file>
@@ -413,19 +431,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>0.802816901408451</v>
+        <v>0.616858237547893</v>
       </c>
       <c r="C2" t="n">
-        <v>0.718232044198895</v>
+        <v>0.676258992805755</v>
       </c>
       <c r="D2" t="n">
-        <v>0.778688524590164</v>
+        <v>0.960199004975124</v>
       </c>
       <c r="E2" t="n">
-        <v>0.695652173913043</v>
+        <v>0.953307392996109</v>
       </c>
       <c r="F2" t="n">
-        <v>0.540890072270825</v>
+        <v>0.655973451327434</v>
       </c>
     </row>
     <row r="3">
@@ -433,19 +451,19 @@
         <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>0.485714285714286</v>
+        <v>0.845559845559846</v>
       </c>
       <c r="C3" t="n">
-        <v>0.527777777777778</v>
+        <v>0.844594594594595</v>
       </c>
       <c r="D3" t="n">
-        <v>0.65625</v>
+        <v>0.869158878504673</v>
       </c>
       <c r="E3" t="n">
-        <v>0.461538461538462</v>
+        <v>0.92057761732852</v>
       </c>
       <c r="F3" t="n">
-        <v>0.490683229813665</v>
+        <v>0.840262582056893</v>
       </c>
     </row>
     <row r="4">
@@ -453,19 +471,19 @@
         <v>8</v>
       </c>
       <c r="B4" t="n">
-        <v>0.783783783783784</v>
+        <v>0.539748953974895</v>
       </c>
       <c r="C4" t="n">
-        <v>0.703703703703704</v>
+        <v>0.815181518151815</v>
       </c>
       <c r="D4" t="n">
-        <v>0.821428571428571</v>
+        <v>0.802690582959641</v>
       </c>
       <c r="E4" t="n">
-        <v>0.857142857142857</v>
+        <v>0.61003861003861</v>
       </c>
       <c r="F4" t="n">
-        <v>0.538805970149254</v>
+        <v>0.803474484256243</v>
       </c>
     </row>
     <row r="5">
@@ -473,19 +491,19 @@
         <v>9</v>
       </c>
       <c r="B5" t="n">
-        <v>0.823529411764706</v>
+        <v>0.895752895752896</v>
       </c>
       <c r="C5" t="n">
-        <v>0.808510638297872</v>
+        <v>0.807817589576547</v>
       </c>
       <c r="D5" t="n">
-        <v>0.882352941176471</v>
+        <v>0.934579439252336</v>
       </c>
       <c r="E5" t="n">
-        <v>0.875</v>
+        <v>0.881294964028777</v>
       </c>
       <c r="F5" t="n">
-        <v>0.55</v>
+        <v>0.88628762541806</v>
       </c>
     </row>
     <row r="6">
@@ -493,19 +511,19 @@
         <v>10</v>
       </c>
       <c r="B6" t="n">
-        <v>0.861111111111111</v>
+        <v>0.686507936507937</v>
       </c>
       <c r="C6" t="n">
-        <v>0.863636363636364</v>
+        <v>0.762345679012346</v>
       </c>
       <c r="D6" t="n">
-        <v>0.785714285714286</v>
+        <v>0.762931034482759</v>
       </c>
       <c r="E6" t="n">
-        <v>0.909090909090909</v>
+        <v>0.807547169811321</v>
       </c>
       <c r="F6" t="n">
-        <v>0.609160305343511</v>
+        <v>0.574786324786325</v>
       </c>
     </row>
     <row r="7">
@@ -513,19 +531,19 @@
         <v>11</v>
       </c>
       <c r="B7" t="n">
-        <v>0.694444444444444</v>
+        <v>0.697247706422018</v>
       </c>
       <c r="C7" t="n">
-        <v>0.53921568627451</v>
+        <v>0.545454545454545</v>
       </c>
       <c r="D7" t="n">
-        <v>0.736842105263158</v>
+        <v>0.684210526315789</v>
       </c>
       <c r="E7" t="n">
-        <v>0.36</v>
+        <v>0.428044280442804</v>
       </c>
       <c r="F7" t="n">
-        <v>0.53353428786737</v>
+        <v>0.598941798941799</v>
       </c>
     </row>
     <row r="8">
@@ -533,19 +551,19 @@
         <v>12</v>
       </c>
       <c r="B8" t="n">
-        <v>0.742857142857143</v>
+        <v>0.65843621399177</v>
       </c>
       <c r="C8" t="n">
-        <v>0.531645569620253</v>
+        <v>0.79672131147541</v>
       </c>
       <c r="D8" t="n">
-        <v>0.784615384615385</v>
+        <v>0.900473933649289</v>
       </c>
       <c r="E8" t="n">
-        <v>0.523809523809524</v>
+        <v>0.786290322580645</v>
       </c>
       <c r="F8" t="n">
-        <v>0.538402457757296</v>
+        <v>0.695966907962771</v>
       </c>
     </row>
     <row r="9">
@@ -553,19 +571,19 @@
         <v>13</v>
       </c>
       <c r="B9" t="n">
-        <v>0.471830985915493</v>
+        <v>0.844444444444444</v>
       </c>
       <c r="C9" t="n">
-        <v>0.56353591160221</v>
+        <v>0.86084142394822</v>
       </c>
       <c r="D9" t="n">
-        <v>0.508196721311475</v>
+        <v>0.800947867298578</v>
       </c>
       <c r="E9" t="n">
-        <v>0.565217391304348</v>
+        <v>0.812</v>
       </c>
       <c r="F9" t="n">
-        <v>0.523291925465838</v>
+        <v>0.813928182807399</v>
       </c>
     </row>
     <row r="10">
@@ -573,19 +591,139 @@
         <v>14</v>
       </c>
       <c r="B10" t="n">
-        <v>0.647887323943662</v>
+        <v>0.581395348837209</v>
       </c>
       <c r="C10" t="n">
-        <v>0.640883977900553</v>
+        <v>0.533546325878594</v>
       </c>
       <c r="D10" t="n">
-        <v>0.622950819672131</v>
+        <v>0.623853211009174</v>
       </c>
       <c r="E10" t="n">
-        <v>0.608695652173913</v>
+        <v>0.690839694656489</v>
       </c>
       <c r="F10" t="n">
-        <v>0.585403726708075</v>
+        <v>0.619895287958115</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.79746835443038</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.776073619631902</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.829596412556054</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.665938864628821</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.760504201680672</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.778156996587031</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.831683168316832</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.858921161825726</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.798553719008264</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.839449541284404</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.8561872909699</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.854077253218884</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.772549019607843</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.717127071823204</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.780392156862745</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.853820598006645</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.847290640394089</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.792307692307692</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.793926247288503</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.788235294117647</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.777003484320557</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.84549356223176</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.743295019157088</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.725690890481064</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.763565891472868</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.752380952380952</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.722943722943723</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.493877551020408</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.5917225950783</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Eu => Europe, gcs_important by vote/support
</commit_message>
<xml_diff>
--- a/xlsx/country_comparison/.xlsx
+++ b/xlsx/country_comparison/.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -35,10 +35,38 @@
     <t xml:space="preserve">United Kingdom</t>
   </si>
   <si>
-    <t xml:space="preserve">Belief about GCS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Belief about NR</t>
+    <t xml:space="preserve">It would succeed in limiting climate change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It would hurt the [Country] economy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It would penalize my household</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It would make people change their lifestyle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It would reduce poverty in low-income countries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It might be detrimental to some poor countries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It could foster global cooperation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It could fuel corruption in low-income countries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It could be subject to fraud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It would be technically difficult to put in place</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Having enough information on
+this scheme and its consequences</t>
   </si>
 </sst>
 </file>
@@ -398,22 +426,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>51.7468893271431</v>
+        <v>0.672053541001286</v>
       </c>
       <c r="C2" t="n">
-        <v>58.7165906294257</v>
+        <v>0.582938067961184</v>
       </c>
       <c r="D2" t="n">
-        <v>61.2471232063537</v>
+        <v>0.540830920916378</v>
       </c>
       <c r="E2" t="n">
-        <v>55.8760774338855</v>
+        <v>0.656789582949536</v>
       </c>
       <c r="F2" t="n">
-        <v>63.2492428282122</v>
+        <v>0.538104795906038</v>
       </c>
       <c r="G2" t="n">
-        <v>56.9303970210785</v>
+        <v>0.541350478300235</v>
       </c>
     </row>
     <row r="3">
@@ -421,22 +449,229 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>55.1540879537179</v>
+        <v>0.891301757279309</v>
       </c>
       <c r="C3" t="n">
-        <v>57.8956679241541</v>
+        <v>0.780204464912827</v>
       </c>
       <c r="D3" t="n">
-        <v>60.3249521322473</v>
+        <v>0.659795214245632</v>
       </c>
       <c r="E3" t="n">
-        <v>53.014236682396</v>
+        <v>0.729457954248223</v>
       </c>
       <c r="F3" t="n">
-        <v>62.0685304640517</v>
+        <v>0.73782451273014</v>
       </c>
       <c r="G3" t="n">
-        <v>59.0733426883397</v>
+        <v>0.902695682752281</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.839128610889381</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.742901276441401</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.7017279146792</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.728815269477337</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.750395530604615</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.782192072002497</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.724595557495586</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.626578181406864</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.658937842683342</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.644915946352901</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.597782105482217</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.580143827052933</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.689054219802248</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.664380381636305</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.704094709238634</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.711275867180752</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.572528055051728</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.60927373973101</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.74503010611439</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.652681493456455</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.646895029917251</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.659443297789059</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.708152559274898</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.636222901700506</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.719660543344661</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.573814842079329</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.523468296219712</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.634321205004898</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.525018018015189</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.562108110779417</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.77708533855146</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.706642015509628</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.782414898061268</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.655380261897868</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.777203628123294</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.689685291309682</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.834418003882785</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.798367178476084</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.775382352209707</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.796236245924259</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.817054675660094</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.794298090146449</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.811160240941621</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.71958710509228</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.697265999422906</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.668537258017323</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.73485497102585</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.740334261560751</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.909620188686539</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.765524000555159</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.784696947296919</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.712068192462401</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.792464056175893</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.791230367967449</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prez, draft (update figures)
</commit_message>
<xml_diff>
--- a/xlsx/country_comparison/.xlsx
+++ b/xlsx/country_comparison/.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -35,27 +35,19 @@
     <t xml:space="preserve">United Kingdom</t>
   </si>
   <si>
-    <t xml:space="preserve">Support for the GCS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Global tax on millionaires</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sharing half of global tax with low-income countries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A maximum wealth limit of $10 billion
-(US) / €100 million (Eu) for each human</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High-income countries funding renewable
-energy in low-income countries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Country]'s foreign aid should be increased</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Universalist</t>
+    <t xml:space="preserve">Global climate scheme (GCS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NR+GCS preferred to NR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C+NR+GCS preferred to C+NR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NR+C preferred to NR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCS+NR preferred to C+NR</t>
   </si>
 </sst>
 </file>
@@ -415,22 +407,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>0.457959991433081</v>
+        <v>0.542040008566919</v>
       </c>
       <c r="C2" t="n">
-        <v>0.242679133235796</v>
+        <v>0.757320866764204</v>
       </c>
       <c r="D2" t="n">
-        <v>0.197154004549498</v>
+        <v>0.802845995450502</v>
       </c>
       <c r="E2" t="n">
-        <v>0.287318534248269</v>
+        <v>0.712681465751731</v>
       </c>
       <c r="F2" t="n">
-        <v>0.190082286886279</v>
+        <v>0.809917713113721</v>
       </c>
       <c r="G2" t="n">
-        <v>0.25893872226297</v>
+        <v>0.74106127773703</v>
       </c>
     </row>
     <row r="3">
@@ -438,22 +430,22 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>0.260397843138756</v>
+        <v>0.546998519360197</v>
       </c>
       <c r="C3" t="n">
-        <v>0.136808410283919</v>
+        <v>0.770223388683434</v>
       </c>
       <c r="D3" t="n">
-        <v>0.132838609114996</v>
+        <v>0.791348238675161</v>
       </c>
       <c r="E3" t="n">
-        <v>0.133317535127324</v>
+        <v>0.7419152210687</v>
       </c>
       <c r="F3" t="n">
-        <v>0.11281931477433</v>
+        <v>0.792397387102864</v>
       </c>
       <c r="G3" t="n">
-        <v>0.141175484791906</v>
+        <v>0.772122341113144</v>
       </c>
     </row>
     <row r="4">
@@ -461,22 +453,22 @@
         <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>0.547746186051635</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.735351301009053</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>0.786517033810842</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.714098080786382</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.782294412865101</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.683359692303094</v>
       </c>
     </row>
     <row r="5">
@@ -484,22 +476,22 @@
         <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>0.389116859621013</v>
+        <v>0.616278518818649</v>
       </c>
       <c r="C5" t="n">
-        <v>0.276479958146891</v>
+        <v>0.840441328944408</v>
       </c>
       <c r="D5" t="n">
-        <v>0.284713606946689</v>
+        <v>0.877676923710508</v>
       </c>
       <c r="E5" t="n">
-        <v>0.292521864346683</v>
+        <v>0.829293481343928</v>
       </c>
       <c r="F5" t="n">
-        <v>0.238985480395989</v>
+        <v>0.8401259487174</v>
       </c>
       <c r="G5" t="n">
-        <v>0.24732684988301</v>
+        <v>0.823739735276932</v>
       </c>
     </row>
     <row r="6">
@@ -507,68 +499,22 @@
         <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>0.245434323397319</v>
+        <v>0.472512715667483</v>
       </c>
       <c r="C6" t="n">
-        <v>0.142248606097258</v>
+        <v>0.515377450158311</v>
       </c>
       <c r="D6" t="n">
-        <v>0.134774093805854</v>
+        <v>0.529174790889353</v>
       </c>
       <c r="E6" t="n">
-        <v>0.149087083860728</v>
+        <v>0.532760503496087</v>
       </c>
       <c r="F6" t="n">
-        <v>0.116451692291737</v>
+        <v>0.490919481564323</v>
       </c>
       <c r="G6" t="n">
-        <v>0.150879564243863</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0.18028384191809</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.138501430842085</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.076424398031436</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.107886976232851</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.104534936604642</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.245975567329776</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0</v>
+        <v>0.520312075113975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>